<commit_message>
[master] Add complete in Review
</commit_message>
<xml_diff>
--- a/reviews/review_points_ZawWinTin.xlsx
+++ b/reviews/review_points_ZawWinTin.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PhuePwintPhway\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Apache24\htdocs\php_training\reviews\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A743C47E-73D2-471C-87F1-1796B0E15973}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9EA7750-33FA-4259-8277-F9AE31DC9D54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Head" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>№</t>
     <phoneticPr fontId="1"/>
@@ -131,6 +131,9 @@
   </si>
   <si>
     <t xml:space="preserve">1) Please write coke format </t>
+  </si>
+  <si>
+    <t>Complete</t>
   </si>
 </sst>
 </file>
@@ -385,6 +388,21 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -402,21 +420,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2172,8 +2175,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15325057-6EF6-4061-BD04-F302EC81437A}">
   <dimension ref="A1:X3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3:H3"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="P2" sqref="P2:U2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2"/>
@@ -2198,30 +2201,30 @@
       <c r="E1" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="18" t="s">
+      <c r="F1" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="19"/>
-      <c r="H1" s="20"/>
-      <c r="I1" s="18" t="s">
+      <c r="G1" s="24"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="19"/>
-      <c r="K1" s="19"/>
-      <c r="L1" s="19"/>
-      <c r="M1" s="19"/>
-      <c r="N1" s="20"/>
+      <c r="J1" s="24"/>
+      <c r="K1" s="24"/>
+      <c r="L1" s="24"/>
+      <c r="M1" s="24"/>
+      <c r="N1" s="25"/>
       <c r="O1" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="P1" s="21" t="s">
+      <c r="P1" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="Q1" s="22"/>
-      <c r="R1" s="22"/>
-      <c r="S1" s="22"/>
-      <c r="T1" s="22"/>
-      <c r="U1" s="23"/>
+      <c r="Q1" s="27"/>
+      <c r="R1" s="27"/>
+      <c r="S1" s="27"/>
+      <c r="T1" s="27"/>
+      <c r="U1" s="28"/>
       <c r="V1" s="13" t="s">
         <v>9</v>
       </c>
@@ -2248,26 +2251,28 @@
       <c r="E2" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="24" t="s">
+      <c r="F2" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="G2" s="24"/>
-      <c r="H2" s="24"/>
-      <c r="I2" s="26" t="s">
+      <c r="G2" s="18"/>
+      <c r="H2" s="18"/>
+      <c r="I2" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="J2" s="27"/>
-      <c r="K2" s="27"/>
-      <c r="L2" s="27"/>
-      <c r="M2" s="27"/>
-      <c r="N2" s="28"/>
+      <c r="J2" s="20"/>
+      <c r="K2" s="20"/>
+      <c r="L2" s="20"/>
+      <c r="M2" s="20"/>
+      <c r="N2" s="21"/>
       <c r="O2" s="12"/>
-      <c r="P2" s="25"/>
-      <c r="Q2" s="25"/>
-      <c r="R2" s="25"/>
-      <c r="S2" s="25"/>
-      <c r="T2" s="25"/>
-      <c r="U2" s="25"/>
+      <c r="P2" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q2" s="22"/>
+      <c r="R2" s="22"/>
+      <c r="S2" s="22"/>
+      <c r="T2" s="22"/>
+      <c r="U2" s="22"/>
       <c r="V2" s="14"/>
       <c r="W2" s="14"/>
       <c r="X2" s="14"/>
@@ -2278,22 +2283,22 @@
       <c r="C3" s="15"/>
       <c r="D3" s="15"/>
       <c r="E3" s="15"/>
-      <c r="F3" s="24"/>
-      <c r="G3" s="24"/>
-      <c r="H3" s="24"/>
-      <c r="I3" s="26"/>
-      <c r="J3" s="27"/>
-      <c r="K3" s="27"/>
-      <c r="L3" s="27"/>
-      <c r="M3" s="27"/>
-      <c r="N3" s="28"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="18"/>
+      <c r="H3" s="18"/>
+      <c r="I3" s="19"/>
+      <c r="J3" s="20"/>
+      <c r="K3" s="20"/>
+      <c r="L3" s="20"/>
+      <c r="M3" s="20"/>
+      <c r="N3" s="21"/>
       <c r="O3" s="12"/>
-      <c r="P3" s="25"/>
-      <c r="Q3" s="25"/>
-      <c r="R3" s="25"/>
-      <c r="S3" s="25"/>
-      <c r="T3" s="25"/>
-      <c r="U3" s="25"/>
+      <c r="P3" s="22"/>
+      <c r="Q3" s="22"/>
+      <c r="R3" s="22"/>
+      <c r="S3" s="22"/>
+      <c r="T3" s="22"/>
+      <c r="U3" s="22"/>
       <c r="V3" s="14"/>
       <c r="W3" s="14"/>
       <c r="X3" s="14"/>
@@ -2310,44 +2315,13 @@
     <mergeCell ref="I2:N2"/>
     <mergeCell ref="P2:U2"/>
   </mergeCells>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:E3 O2:O3 W2:W3" xr:uid="{3ACB177A-5336-4683-B2DE-950F5C248407}">
+      <formula1>#REF!</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="5">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{3ACB177A-5336-4683-B2DE-950F5C248407}">
-          <x14:formula1>
-            <xm:f>#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>C2:C3</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{FE880F0B-4C2C-45F4-9766-4F1DCDF32C0D}">
-          <x14:formula1>
-            <xm:f>#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>W2:W3</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{C1637462-1934-4170-A1C6-316A3BB2142F}">
-          <x14:formula1>
-            <xm:f>#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>O2:O3</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{780D1ED1-8618-4BF4-8D00-DC10E6336C97}">
-          <x14:formula1>
-            <xm:f>#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>E2:E3</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{364060D2-DDC1-4FA8-9A27-0C8A5FAFA12D}">
-          <x14:formula1>
-            <xm:f>#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>D2:D3</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -3651,7 +3625,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C20C7AB-7563-4C9A-AC10-EBD0C653D27E}">
   <dimension ref="A1:N26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
[master] Update Review Points
</commit_message>
<xml_diff>
--- a/reviews/review_points_ZawWinTin.xlsx
+++ b/reviews/review_points_ZawWinTin.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Apache24\htdocs\php_training\reviews\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zaw Win Tin\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9EA7750-33FA-4259-8277-F9AE31DC9D54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28596169-D5AA-4B89-B38B-C5BD6C3CD3F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Head" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="tutorial-7" sheetId="9" r:id="rId5"/>
     <sheet name="tutorial-8" sheetId="10" r:id="rId6"/>
     <sheet name="tutorial-9" sheetId="11" r:id="rId7"/>
+    <sheet name="tutorial-10" sheetId="12" r:id="rId8"/>
   </sheets>
   <calcPr calcId="145621"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>№</t>
     <phoneticPr fontId="1"/>
@@ -130,7 +131,10 @@
     <t>code format</t>
   </si>
   <si>
-    <t xml:space="preserve">1) Please write coke format </t>
+    <t>Phue Pwint Phway</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) Please write code format </t>
   </si>
   <si>
     <t>Complete</t>
@@ -140,7 +144,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -157,6 +161,12 @@
     <font>
       <sz val="9"/>
       <color theme="1"/>
+      <name val="Meiryo"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
       <name val="Meiryo"/>
       <family val="2"/>
     </font>
@@ -333,7 +343,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -387,6 +397,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -443,13 +456,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>276225</xdr:colOff>
+      <xdr:colOff>390525</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>190500</xdr:colOff>
+      <xdr:colOff>304800</xdr:colOff>
       <xdr:row>20</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
@@ -466,8 +479,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1647825" y="838200"/>
-          <a:ext cx="6086475" cy="2628900"/>
+          <a:off x="1609725" y="822960"/>
+          <a:ext cx="5400675" cy="2567940"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -535,7 +548,30 @@
             </a:rPr>
             <a:t>Zaw Win Tin</a:t>
           </a:r>
-          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="2000">
+        </a:p>
+        <a:p>
+          <a:pPr algn="r"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="800">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Meiryo" panose="020B0604030504040204" pitchFamily="34" charset="-128"/>
+              <a:ea typeface="Meiryo" panose="020B0604030504040204" pitchFamily="34" charset="-128"/>
+            </a:rPr>
+            <a:t>reviewer</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="800" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Meiryo" panose="020B0604030504040204" pitchFamily="34" charset="-128"/>
+              <a:ea typeface="Meiryo" panose="020B0604030504040204" pitchFamily="34" charset="-128"/>
+            </a:rPr>
+            <a:t> =&gt; Phue Pwint Phway</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="800">
             <a:solidFill>
               <a:sysClr val="windowText" lastClr="000000"/>
             </a:solidFill>
@@ -1009,6 +1045,88 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Rectangle 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{50ED6357-4E85-44F3-AD1E-EDFA5144362E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1495425" y="822960"/>
+          <a:ext cx="5400675" cy="2567940"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent6"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="2800">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Meiryo" panose="020B0604030504040204" pitchFamily="34" charset="-128"/>
+              <a:ea typeface="Meiryo" panose="020B0604030504040204" pitchFamily="34" charset="-128"/>
+            </a:rPr>
+            <a:t>All OK</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office テーマ">
   <a:themeElements>
@@ -1309,7 +1427,7 @@
   <dimension ref="A1:N26"/>
   <sheetViews>
     <sheetView view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="B12" sqref="A1:XFD1048576"/>
+      <selection activeCell="N19" sqref="N19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2"/>
@@ -2175,7 +2293,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15325057-6EF6-4061-BD04-F302EC81437A}">
   <dimension ref="A1:X3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
       <selection activeCell="P2" sqref="P2:U2"/>
     </sheetView>
   </sheetViews>
@@ -2183,6 +2301,7 @@
   <cols>
     <col min="2" max="2" width="10.5546875" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="54.77734375" customWidth="1"/>
+    <col min="15" max="15" width="25.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="30">
@@ -2201,30 +2320,30 @@
       <c r="E1" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="23" t="s">
+      <c r="F1" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="24"/>
-      <c r="H1" s="25"/>
-      <c r="I1" s="23" t="s">
+      <c r="G1" s="25"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="24"/>
-      <c r="K1" s="24"/>
-      <c r="L1" s="24"/>
-      <c r="M1" s="24"/>
-      <c r="N1" s="25"/>
+      <c r="J1" s="25"/>
+      <c r="K1" s="25"/>
+      <c r="L1" s="25"/>
+      <c r="M1" s="25"/>
+      <c r="N1" s="26"/>
       <c r="O1" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="P1" s="26" t="s">
+      <c r="P1" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="Q1" s="27"/>
-      <c r="R1" s="27"/>
-      <c r="S1" s="27"/>
-      <c r="T1" s="27"/>
-      <c r="U1" s="28"/>
+      <c r="Q1" s="28"/>
+      <c r="R1" s="28"/>
+      <c r="S1" s="28"/>
+      <c r="T1" s="28"/>
+      <c r="U1" s="29"/>
       <c r="V1" s="13" t="s">
         <v>9</v>
       </c>
@@ -2251,28 +2370,30 @@
       <c r="E2" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="18" t="s">
+      <c r="F2" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="G2" s="18"/>
-      <c r="H2" s="18"/>
-      <c r="I2" s="19" t="s">
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" s="21"/>
+      <c r="K2" s="21"/>
+      <c r="L2" s="21"/>
+      <c r="M2" s="21"/>
+      <c r="N2" s="22"/>
+      <c r="O2" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="J2" s="20"/>
-      <c r="K2" s="20"/>
-      <c r="L2" s="20"/>
-      <c r="M2" s="20"/>
-      <c r="N2" s="21"/>
-      <c r="O2" s="12"/>
-      <c r="P2" s="22" t="s">
-        <v>17</v>
+      <c r="P2" s="23" t="s">
+        <v>18</v>
       </c>
-      <c r="Q2" s="22"/>
-      <c r="R2" s="22"/>
-      <c r="S2" s="22"/>
-      <c r="T2" s="22"/>
-      <c r="U2" s="22"/>
+      <c r="Q2" s="23"/>
+      <c r="R2" s="23"/>
+      <c r="S2" s="23"/>
+      <c r="T2" s="23"/>
+      <c r="U2" s="23"/>
       <c r="V2" s="14"/>
       <c r="W2" s="14"/>
       <c r="X2" s="14"/>
@@ -2283,22 +2404,22 @@
       <c r="C3" s="15"/>
       <c r="D3" s="15"/>
       <c r="E3" s="15"/>
-      <c r="F3" s="18"/>
-      <c r="G3" s="18"/>
-      <c r="H3" s="18"/>
-      <c r="I3" s="19"/>
-      <c r="J3" s="20"/>
-      <c r="K3" s="20"/>
-      <c r="L3" s="20"/>
-      <c r="M3" s="20"/>
-      <c r="N3" s="21"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="19"/>
+      <c r="I3" s="20"/>
+      <c r="J3" s="21"/>
+      <c r="K3" s="21"/>
+      <c r="L3" s="21"/>
+      <c r="M3" s="21"/>
+      <c r="N3" s="22"/>
       <c r="O3" s="12"/>
-      <c r="P3" s="22"/>
-      <c r="Q3" s="22"/>
-      <c r="R3" s="22"/>
-      <c r="S3" s="22"/>
-      <c r="T3" s="22"/>
-      <c r="U3" s="22"/>
+      <c r="P3" s="23"/>
+      <c r="Q3" s="23"/>
+      <c r="R3" s="23"/>
+      <c r="S3" s="23"/>
+      <c r="T3" s="23"/>
+      <c r="U3" s="23"/>
       <c r="V3" s="14"/>
       <c r="W3" s="14"/>
       <c r="X3" s="14"/>
@@ -2316,12 +2437,13 @@
     <mergeCell ref="P2:U2"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:E3 O2:O3 W2:W3" xr:uid="{3ACB177A-5336-4683-B2DE-950F5C248407}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="W2:W3 C2:E3 O3" xr:uid="{3ACB177A-5336-4683-B2DE-950F5C248407}">
       <formula1>#REF!</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -3194,7 +3316,7 @@
   <dimension ref="A1:N26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2"/>
@@ -4051,4 +4173,436 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90CF68F5-3E66-4BFC-8BB6-68791142067D}">
+  <dimension ref="A1:N26"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H25" sqref="H25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.2"/>
+  <sheetData>
+    <row r="1" spans="1:14">
+      <c r="A1" s="1"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="3"/>
+    </row>
+    <row r="2" spans="1:14">
+      <c r="A2" s="4"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="6"/>
+    </row>
+    <row r="3" spans="1:14">
+      <c r="A3" s="4"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5"/>
+      <c r="L3" s="5"/>
+      <c r="M3" s="5"/>
+      <c r="N3" s="6"/>
+    </row>
+    <row r="4" spans="1:14">
+      <c r="A4" s="4"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="5"/>
+      <c r="L4" s="5"/>
+      <c r="M4" s="5"/>
+      <c r="N4" s="6"/>
+    </row>
+    <row r="5" spans="1:14">
+      <c r="A5" s="4"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="5"/>
+      <c r="K5" s="5"/>
+      <c r="L5" s="5"/>
+      <c r="M5" s="5"/>
+      <c r="N5" s="6"/>
+    </row>
+    <row r="6" spans="1:14">
+      <c r="A6" s="4"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="5"/>
+      <c r="K6" s="5"/>
+      <c r="L6" s="5"/>
+      <c r="M6" s="5"/>
+      <c r="N6" s="6"/>
+    </row>
+    <row r="7" spans="1:14">
+      <c r="A7" s="4"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
+      <c r="J7" s="5"/>
+      <c r="K7" s="5"/>
+      <c r="L7" s="5"/>
+      <c r="M7" s="5"/>
+      <c r="N7" s="6"/>
+    </row>
+    <row r="8" spans="1:14">
+      <c r="A8" s="4"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="5"/>
+      <c r="J8" s="5"/>
+      <c r="K8" s="5"/>
+      <c r="L8" s="5"/>
+      <c r="M8" s="5"/>
+      <c r="N8" s="6"/>
+    </row>
+    <row r="9" spans="1:14">
+      <c r="A9" s="4"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="5"/>
+      <c r="K9" s="5"/>
+      <c r="L9" s="5"/>
+      <c r="M9" s="5"/>
+      <c r="N9" s="6"/>
+    </row>
+    <row r="10" spans="1:14">
+      <c r="A10" s="4"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="5"/>
+      <c r="J10" s="5"/>
+      <c r="K10" s="5"/>
+      <c r="L10" s="5"/>
+      <c r="M10" s="5"/>
+      <c r="N10" s="6"/>
+    </row>
+    <row r="11" spans="1:14">
+      <c r="A11" s="4"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
+      <c r="I11" s="5"/>
+      <c r="J11" s="5"/>
+      <c r="K11" s="5"/>
+      <c r="L11" s="5"/>
+      <c r="M11" s="5"/>
+      <c r="N11" s="6"/>
+    </row>
+    <row r="12" spans="1:14">
+      <c r="A12" s="4"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="5"/>
+      <c r="J12" s="5"/>
+      <c r="K12" s="5"/>
+      <c r="L12" s="5"/>
+      <c r="M12" s="5"/>
+      <c r="N12" s="6"/>
+    </row>
+    <row r="13" spans="1:14">
+      <c r="A13" s="4"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="5"/>
+      <c r="J13" s="5"/>
+      <c r="K13" s="5"/>
+      <c r="L13" s="5"/>
+      <c r="M13" s="5"/>
+      <c r="N13" s="6"/>
+    </row>
+    <row r="14" spans="1:14">
+      <c r="A14" s="4"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
+      <c r="I14" s="5"/>
+      <c r="J14" s="5"/>
+      <c r="K14" s="5"/>
+      <c r="L14" s="5"/>
+      <c r="M14" s="5"/>
+      <c r="N14" s="6"/>
+    </row>
+    <row r="15" spans="1:14">
+      <c r="A15" s="4"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5"/>
+      <c r="I15" s="5"/>
+      <c r="J15" s="5"/>
+      <c r="K15" s="5"/>
+      <c r="L15" s="5"/>
+      <c r="M15" s="5"/>
+      <c r="N15" s="6"/>
+    </row>
+    <row r="16" spans="1:14">
+      <c r="A16" s="4"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="5"/>
+      <c r="I16" s="5"/>
+      <c r="J16" s="5"/>
+      <c r="K16" s="5"/>
+      <c r="L16" s="5"/>
+      <c r="M16" s="5"/>
+      <c r="N16" s="6"/>
+    </row>
+    <row r="17" spans="1:14">
+      <c r="A17" s="4"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="5"/>
+      <c r="H17" s="5"/>
+      <c r="I17" s="5"/>
+      <c r="J17" s="5"/>
+      <c r="K17" s="5"/>
+      <c r="L17" s="5"/>
+      <c r="M17" s="5"/>
+      <c r="N17" s="6"/>
+    </row>
+    <row r="18" spans="1:14">
+      <c r="A18" s="4"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="5"/>
+      <c r="I18" s="5"/>
+      <c r="J18" s="5"/>
+      <c r="K18" s="5"/>
+      <c r="L18" s="5"/>
+      <c r="M18" s="5"/>
+      <c r="N18" s="6"/>
+    </row>
+    <row r="19" spans="1:14">
+      <c r="A19" s="4"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="5"/>
+      <c r="H19" s="5"/>
+      <c r="I19" s="5"/>
+      <c r="J19" s="5"/>
+      <c r="K19" s="5"/>
+      <c r="L19" s="5"/>
+      <c r="M19" s="5"/>
+      <c r="N19" s="6"/>
+    </row>
+    <row r="20" spans="1:14">
+      <c r="A20" s="4"/>
+      <c r="B20" s="5"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="5"/>
+      <c r="H20" s="5"/>
+      <c r="I20" s="5"/>
+      <c r="J20" s="5"/>
+      <c r="K20" s="5"/>
+      <c r="L20" s="5"/>
+      <c r="M20" s="5"/>
+      <c r="N20" s="6"/>
+    </row>
+    <row r="21" spans="1:14">
+      <c r="A21" s="4"/>
+      <c r="B21" s="5"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="5"/>
+      <c r="H21" s="5"/>
+      <c r="I21" s="5"/>
+      <c r="J21" s="5"/>
+      <c r="K21" s="5"/>
+      <c r="L21" s="5"/>
+      <c r="M21" s="5"/>
+      <c r="N21" s="6"/>
+    </row>
+    <row r="22" spans="1:14">
+      <c r="A22" s="4"/>
+      <c r="B22" s="5"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="5"/>
+      <c r="H22" s="5"/>
+      <c r="I22" s="5"/>
+      <c r="J22" s="5"/>
+      <c r="K22" s="5"/>
+      <c r="L22" s="5"/>
+      <c r="M22" s="5"/>
+      <c r="N22" s="6"/>
+    </row>
+    <row r="23" spans="1:14">
+      <c r="A23" s="4"/>
+      <c r="B23" s="5"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
+      <c r="G23" s="5"/>
+      <c r="H23" s="5"/>
+      <c r="I23" s="5"/>
+      <c r="J23" s="5"/>
+      <c r="K23" s="5"/>
+      <c r="L23" s="5"/>
+      <c r="M23" s="5"/>
+      <c r="N23" s="6"/>
+    </row>
+    <row r="24" spans="1:14">
+      <c r="A24" s="4"/>
+      <c r="B24" s="5"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
+      <c r="G24" s="5"/>
+      <c r="H24" s="5"/>
+      <c r="I24" s="5"/>
+      <c r="J24" s="5"/>
+      <c r="K24" s="5"/>
+      <c r="L24" s="5"/>
+      <c r="M24" s="5"/>
+      <c r="N24" s="6"/>
+    </row>
+    <row r="25" spans="1:14">
+      <c r="A25" s="4"/>
+      <c r="B25" s="5"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="5"/>
+      <c r="G25" s="5"/>
+      <c r="H25" s="5"/>
+      <c r="I25" s="5"/>
+      <c r="J25" s="5"/>
+      <c r="K25" s="5"/>
+      <c r="L25" s="5"/>
+      <c r="M25" s="5"/>
+      <c r="N25" s="6"/>
+    </row>
+    <row r="26" spans="1:14">
+      <c r="A26" s="7"/>
+      <c r="B26" s="8"/>
+      <c r="C26" s="8"/>
+      <c r="D26" s="8"/>
+      <c r="E26" s="8"/>
+      <c r="F26" s="8"/>
+      <c r="G26" s="8"/>
+      <c r="H26" s="8"/>
+      <c r="I26" s="8"/>
+      <c r="J26" s="8"/>
+      <c r="K26" s="8"/>
+      <c r="L26" s="8"/>
+      <c r="M26" s="8"/>
+      <c r="N26" s="9"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>